<commit_message>
fixes rule_name in scrapers and gets content also
</commit_message>
<xml_diff>
--- a/output/excel/income_tax_rules.xlsx
+++ b/output/excel/income_tax_rules.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rule - 1</t>
+          <t>rule_1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rule - 2</t>
+          <t>rule_2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rule - 2A</t>
+          <t>rule_2a</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rule - 2B</t>
+          <t>rule_2b</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rule - 2BA</t>
+          <t>rule_2ba</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rule - 2BB</t>
+          <t>rule_2bb</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rule - 2BBA</t>
+          <t>rule_2bba</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rule - 2BBB</t>
+          <t>rule_2bbb</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rule - 2BC</t>
+          <t>rule_2bc</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rule - 2C</t>
+          <t>rule_2c</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rule - 2D</t>
+          <t>rule_2d</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rule - 2DA</t>
+          <t>rule_2da</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rule - 2DAA</t>
+          <t>rule_2daa</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Rule - 2DB</t>
+          <t>rule_2db</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Rule - 2DC</t>
+          <t>rule_2dc</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rule - 2DCA</t>
+          <t>rule_2dca</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Rule - 2DD</t>
+          <t>rule_2dd</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rule - 2E</t>
+          <t>rule_2e</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Rule - 2F</t>
+          <t>rule_2f</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rule - 3</t>
+          <t>rule_3</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rule - 3A</t>
+          <t>rule_3a</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Rule - 3B</t>
+          <t>rule_3b</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Rule - 4</t>
+          <t>rule_4</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Rule - 5</t>
+          <t>rule_5</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rule - 5A</t>
+          <t>rule_5a</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Rule - 5AA</t>
+          <t>rule_5aa</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Rule - 5AB</t>
+          <t>rule_5ab</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Rule - 5AC</t>
+          <t>rule_5ac</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Rule - 5AD</t>
+          <t>rule_5ad</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Rule - 5B</t>
+          <t>rule_5b</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Rule - 5C</t>
+          <t>rule_5c</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Rule - 5CA</t>
+          <t>rule_5ca</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Rule - 5D</t>
+          <t>rule_5d</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Rule - 5E</t>
+          <t>rule_5e</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Rule - 5F</t>
+          <t>rule_5f</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Rule - 5G</t>
+          <t>rule_5g</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Rule - 6</t>
+          <t>rule_6</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Rule - 6A</t>
+          <t>rule_6a</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Rule - 6AA</t>
+          <t>rule_6aa</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Rule - 6AAA</t>
+          <t>rule_6aaa</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Rule - 6AAB</t>
+          <t>rule_6aab</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Rule - 6AAC</t>
+          <t>rule_6aac</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Rule - 6AAD</t>
+          <t>rule_6aad</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Rule - 6AAE</t>
+          <t>rule_6aae</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Rule - 6AAF</t>
+          <t>rule_6aaf</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Rule - 6AAG</t>
+          <t>rule_6aag</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Rule - 6AAH</t>
+          <t>rule_6aah</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Rule - 6AB</t>
+          <t>rule_6ab</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Rule - 6ABA</t>
+          <t>rule_6aba</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Rule - 6ABAA</t>
+          <t>rule_6abaa</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Rule - 6ABB</t>
+          <t>rule_6abb</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Rule - 6ABBA</t>
+          <t>rule_6abba</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Rule - 6ABBB</t>
+          <t>rule_6abbb</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Rule - 6AC</t>
+          <t>rule_6ac</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Rule - 6B</t>
+          <t>rule_6b</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Rule - 6C</t>
+          <t>rule_6c</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rule - 6D</t>
+          <t>rule_6d</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Rule - 6DD</t>
+          <t>rule_6dd</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Rule - 6DDA</t>
+          <t>rule_6dda</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Rule - 6DDB</t>
+          <t>rule_6ddb</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Rule - 6DDC</t>
+          <t>rule_6ddc</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Rule - 6DDD</t>
+          <t>rule_6ddd</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Rule - 6E</t>
+          <t>rule_6e</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Rule - 6EA</t>
+          <t>rule_6ea</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Rule - 6EB</t>
+          <t>rule_6eb</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Rule - 6F</t>
+          <t>rule_6f</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Rule - 6G</t>
+          <t>rule_6g</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Rule - 6GA</t>
+          <t>rule_6ga</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Rule - 6GB</t>
+          <t>rule_6gb</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Rule - 6H</t>
+          <t>rule_6h</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Rule - 7</t>
+          <t>rule_7</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Rule - 7A</t>
+          <t>rule_7a</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Rule - 7B</t>
+          <t>rule_7b</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2663,7 +2663,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Rule - 8</t>
+          <t>rule_8</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Rule - 8A</t>
+          <t>rule_8a</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Rule - 8AA</t>
+          <t>rule_8aa</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Rule - 8AB</t>
+          <t>rule_8ab</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Rule - 8AC</t>
+          <t>rule_8ac</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Rule - 8AD</t>
+          <t>rule_8ad</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Rule - 8B</t>
+          <t>rule_8b</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Rule - 8C</t>
+          <t>rule_8c</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Rule - 8D</t>
+          <t>rule_8d</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Rule - 9</t>
+          <t>rule_9</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Rule - 9A</t>
+          <t>rule_9a</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Rule - 9B</t>
+          <t>rule_9b</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Rule - 9C</t>
+          <t>rule_9c</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Rule - 9D</t>
+          <t>rule_9d</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Rule - 10</t>
+          <t>rule_10</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Rule - 10A</t>
+          <t>rule_10a</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Rule - 10AB</t>
+          <t>rule_10ab</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Rule - 10B</t>
+          <t>rule_10b</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Rule - 10C</t>
+          <t>rule_10c</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Rule - 10CA</t>
+          <t>rule_10ca</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Rule - 10CB</t>
+          <t>rule_10cb</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Rule - 10D</t>
+          <t>rule_10d</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Rule - 10DA</t>
+          <t>rule_10da</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Rule - 10DB</t>
+          <t>rule_10db</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Rule - 10E</t>
+          <t>rule_10e</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Rule - 10F</t>
+          <t>rule_10f</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Rule - 10G</t>
+          <t>rule_10g</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Rule - 10H</t>
+          <t>rule_10h</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Rule - 10-I</t>
+          <t>rule_10</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Rule - 10J</t>
+          <t>rule_10j</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Rule - 10K</t>
+          <t>rule_10k</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Rule - 10L</t>
+          <t>rule_10l</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Rule - 10M</t>
+          <t>rule_10m</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Rule - 10MA</t>
+          <t>rule_10ma</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Rule - 10N</t>
+          <t>rule_10n</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Rule - 10-O</t>
+          <t>rule_10</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Rule - 10P</t>
+          <t>rule_10p</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Rule - 10Q</t>
+          <t>rule_10q</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Rule - 10R</t>
+          <t>rule_10r</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Rule - 10RA</t>
+          <t>rule_10ra</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Rule - 10RB</t>
+          <t>rule_10rb</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Rule - 10S</t>
+          <t>rule_10s</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Rule - 10T</t>
+          <t>rule_10t</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Rule - 10TA</t>
+          <t>rule_10ta</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Rule - 10TB</t>
+          <t>rule_10tb</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Rule - 10TC</t>
+          <t>rule_10tc</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Rule - 10TD</t>
+          <t>rule_10td</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Rule - 10TE</t>
+          <t>rule_10te</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Rule - 10TF</t>
+          <t>rule_10tf</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Rule - 10TG</t>
+          <t>rule_10tg</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Rule - 10TH</t>
+          <t>rule_10th</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Rule - 10THA</t>
+          <t>rule_10tha</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Rule - 10THB</t>
+          <t>rule_10thb</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Rule - 10THC</t>
+          <t>rule_10thc</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Rule - 10THD</t>
+          <t>rule_10thd</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Rule - 10TI</t>
+          <t>rule_10ti</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4343,7 +4343,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Rule - 10TIA</t>
+          <t>rule_10tia</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Rule - 10TIB</t>
+          <t>rule_10tib</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Rule - 10TIC</t>
+          <t>rule_10tic</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4433,7 +4433,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Rule - 10U</t>
+          <t>rule_10u</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Rule - 10UA</t>
+          <t>rule_10ua</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Rule - 10UB</t>
+          <t>rule_10ub</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Rule - 10UC</t>
+          <t>rule_10uc</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Rule - 10UD</t>
+          <t>rule_10ud</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4583,7 +4583,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Rule - 10UE</t>
+          <t>rule_10ue</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Rule - 10UF</t>
+          <t>rule_10uf</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Rule - 10V</t>
+          <t>rule_10v</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Rule - 10VA</t>
+          <t>rule_10va</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4703,7 +4703,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Rule - 10VB</t>
+          <t>rule_10vb</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Rule - 11</t>
+          <t>rule_11</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Rule - 11A</t>
+          <t>rule_11a</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Rule - 11AA</t>
+          <t>rule_11aa</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Rule - 11B</t>
+          <t>rule_11b</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Rule - 11C</t>
+          <t>rule_11c</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4883,7 +4883,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Rule - 11D</t>
+          <t>rule_11d</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Rule - 11DD</t>
+          <t>rule_11dd</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Rule - 11E</t>
+          <t>rule_11e</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Rule - 11EA</t>
+          <t>rule_11ea</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -5003,7 +5003,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Rule - 11EE</t>
+          <t>rule_11ee</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5033,7 +5033,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Rule - 11F</t>
+          <t>rule_11f</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Rule - 11G</t>
+          <t>rule_11g</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Rule - 11H</t>
+          <t>rule_11h</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Rule - 11-I</t>
+          <t>rule_11</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Rule - 11J</t>
+          <t>rule_11j</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Rule - 11K</t>
+          <t>rule_11k</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5213,7 +5213,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Rule - 11L</t>
+          <t>rule_11l</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Rule - 11M</t>
+          <t>rule_11m</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -5273,7 +5273,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Rule - 11MA</t>
+          <t>rule_11ma</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5303,7 +5303,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Rule - 11MAA</t>
+          <t>rule_11maa</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Rule - 11N</t>
+          <t>rule_11n</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Rule - 11-O</t>
+          <t>rule_11</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Rule - 11-OA</t>
+          <t>rule_11</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Rule - 11-OB</t>
+          <t>rule_11</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Rule - 11P</t>
+          <t>rule_11p</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5483,7 +5483,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Rule - 11Q</t>
+          <t>rule_11q</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Rule - 11R</t>
+          <t>rule_11r</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Rule - 11S</t>
+          <t>rule_11s</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Rule - 11T</t>
+          <t>rule_11t</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5603,7 +5603,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Rule - 11U</t>
+          <t>rule_11u</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Rule - 11UA</t>
+          <t>rule_11ua</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Rule - 11UAA</t>
+          <t>rule_11uaa</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5693,7 +5693,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Rule - 11UAB</t>
+          <t>rule_11uab</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -5723,7 +5723,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Rule - 11UAC</t>
+          <t>rule_11uac</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Rule - 11UACA</t>
+          <t>rule_11uaca</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Rule - 11UAD</t>
+          <t>rule_11uad</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Rule - 11UAE</t>
+          <t>rule_11uae</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -5843,7 +5843,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Rule - 11UB</t>
+          <t>rule_11ub</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Rule - 11UC</t>
+          <t>rule_11uc</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Rule - 11UD</t>
+          <t>rule_11ud</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Rule - 11UE</t>
+          <t>rule_11ue</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Rule - 11UF</t>
+          <t>rule_11uf</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5993,7 +5993,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Rule - 12</t>
+          <t>rule_12</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Rule - 12A</t>
+          <t>rule_12a</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -6053,7 +6053,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Rule - 12AA</t>
+          <t>rule_12aa</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Rule - 12AB</t>
+          <t>rule_12ab</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -6113,7 +6113,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Rule - 12AC</t>
+          <t>rule_12ac</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -6143,7 +6143,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Rule - 12AD</t>
+          <t>rule_12ad</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Rule - 12AE</t>
+          <t>rule_12ae</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Rule - 12B</t>
+          <t>rule_12b</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Rule - 12BA</t>
+          <t>rule_12ba</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Rule - 12C</t>
+          <t>rule_12c</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Rule - 12CA</t>
+          <t>rule_12ca</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Rule - 12CB</t>
+          <t>rule_12cb</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -6353,7 +6353,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Rule - 12CC</t>
+          <t>rule_12cc</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Rule - 12D</t>
+          <t>rule_12d</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Rule - 12E</t>
+          <t>rule_12e</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Rule - 12F</t>
+          <t>rule_12f</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Rule - 13</t>
+          <t>rule_13</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Rule - 13A</t>
+          <t>rule_13a</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Rule - 14</t>
+          <t>rule_14</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -6563,7 +6563,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Rule - 14A</t>
+          <t>rule_14a</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Rule - 14B</t>
+          <t>rule_14b</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -6623,7 +6623,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Rule - 14C</t>
+          <t>rule_14c</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -6653,7 +6653,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Rule - 15</t>
+          <t>rule_15</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Rule - 15A</t>
+          <t>rule_15a</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Rule - 16</t>
+          <t>rule_16</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -6743,7 +6743,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Rule - 16A</t>
+          <t>rule_16a</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Rule - 16B</t>
+          <t>rule_16b</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Rule - 16C</t>
+          <t>rule_16c</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Rule - 16CC</t>
+          <t>rule_16cc</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Rule - 16D</t>
+          <t>rule_16d</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -6893,7 +6893,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Rule - 16DD</t>
+          <t>rule_16dd</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -6923,7 +6923,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Rule - 16E</t>
+          <t>rule_16e</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -6953,7 +6953,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Rule - 16F</t>
+          <t>rule_16f</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -6983,7 +6983,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Rule - 17</t>
+          <t>rule_17</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Rule - 17A</t>
+          <t>rule_17a</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Rule - 17AA</t>
+          <t>rule_17aa</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -7073,7 +7073,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Rule - 17B</t>
+          <t>rule_17b</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Rule - 17C</t>
+          <t>rule_17c</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Rule - 17CA</t>
+          <t>rule_17ca</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -7163,7 +7163,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Rule - 17CB</t>
+          <t>rule_17cb</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -7193,7 +7193,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Rule - 17D</t>
+          <t>rule_17d</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Rule - 18</t>
+          <t>rule_18</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -7253,7 +7253,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Rule - 18A</t>
+          <t>rule_18a</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -7283,7 +7283,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Rule - 18AA</t>
+          <t>rule_18aa</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -7313,7 +7313,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Rule - 18AAA</t>
+          <t>rule_18aaa</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -7343,7 +7343,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Rule - 18AAAA</t>
+          <t>rule_18aaaa</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -7373,7 +7373,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Rule - 18AAAAA</t>
+          <t>rule_18aaaaa</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -7403,7 +7403,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Rule - 18AAB</t>
+          <t>rule_18aab</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7433,7 +7433,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Rule - 18AB</t>
+          <t>rule_18ab</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Rule - 18B</t>
+          <t>rule_18b</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Rule - 18BB</t>
+          <t>rule_18bb</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Rule - 18BBA</t>
+          <t>rule_18bba</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -7553,7 +7553,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Rule - 18BBB</t>
+          <t>rule_18bbb</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -7583,7 +7583,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Rule - 18BBC</t>
+          <t>rule_18bbc</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Rule - 18BBD</t>
+          <t>rule_18bbd</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -7643,7 +7643,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Rule - 18BBE</t>
+          <t>rule_18bbe</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -7673,7 +7673,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Rule - 18C</t>
+          <t>rule_18c</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Rule - 18D</t>
+          <t>rule_18d</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -7733,7 +7733,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Rule - 18DA</t>
+          <t>rule_18da</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -7763,7 +7763,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Rule - 18DB</t>
+          <t>rule_18db</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -7793,7 +7793,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Rule - 18DC</t>
+          <t>rule_18dc</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -7823,7 +7823,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Rule - 18DD</t>
+          <t>rule_18dd</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -7853,7 +7853,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Rule - 18DDA</t>
+          <t>rule_18dda</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -7883,7 +7883,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Rule - 18DE</t>
+          <t>rule_18de</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Rule - 19</t>
+          <t>rule_19</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -7943,7 +7943,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Rule - 19A</t>
+          <t>rule_19a</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -7973,7 +7973,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Rule - 19AB</t>
+          <t>rule_19ab</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Rule - 19AC</t>
+          <t>rule_19ac</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Rule - 19AD</t>
+          <t>rule_19ad</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Rule - 19AE</t>
+          <t>rule_19ae</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -8093,7 +8093,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Rule - 20</t>
+          <t>rule_20</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -8123,7 +8123,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Rule - 20A</t>
+          <t>rule_20a</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -8153,7 +8153,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Rule - 20AB</t>
+          <t>rule_20ab</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -8183,7 +8183,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Rule - 21</t>
+          <t>rule_21</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -8213,7 +8213,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Rule - 21A</t>
+          <t>rule_21a</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -8243,7 +8243,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Rule - 21AA</t>
+          <t>rule_21aa</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Rule - 21AAA</t>
+          <t>rule_21aaa</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Rule - 21AB</t>
+          <t>rule_21ab</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -8333,7 +8333,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Rule - 21AC</t>
+          <t>rule_21ac</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8363,7 +8363,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Rule - 21ACA</t>
+          <t>rule_21aca</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -8393,7 +8393,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Rule - 21AD</t>
+          <t>rule_21ad</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -8423,7 +8423,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Rule - 21AE</t>
+          <t>rule_21ae</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -8453,7 +8453,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Rule - 21AF</t>
+          <t>rule_21af</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Rule - 21AG</t>
+          <t>rule_21ag</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -8513,7 +8513,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Rule - 21AGA</t>
+          <t>rule_21aga</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -8543,7 +8543,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Rule - 21AH</t>
+          <t>rule_21ah</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -8573,7 +8573,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Rule - 21AHA</t>
+          <t>rule_21aha</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -8603,7 +8603,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Rule - 21AI</t>
+          <t>rule_21ai</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -8633,7 +8633,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Rule - 21AIA</t>
+          <t>rule_21aia</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -8663,7 +8663,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Rule - 21AJ</t>
+          <t>rule_21aj</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -8693,7 +8693,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Rule - 21AJA</t>
+          <t>rule_21aja</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -8723,7 +8723,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Rule - 21AJAA</t>
+          <t>rule_21ajaa</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Rule - 21AK</t>
+          <t>rule_21ak</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Rule - 21AL</t>
+          <t>rule_21al</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -8813,7 +8813,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Rule - 21B</t>
+          <t>rule_21b</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -8843,7 +8843,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Rule - 22</t>
+          <t>rule_22</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -8873,7 +8873,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Rule - 23</t>
+          <t>rule_23</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -8903,7 +8903,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Rule - 24</t>
+          <t>rule_24</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -8933,7 +8933,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Rule - 24A</t>
+          <t>rule_24a</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Rule - 25</t>
+          <t>rule_25</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -8993,7 +8993,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Rule - 26</t>
+          <t>rule_26</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9023,7 +9023,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Rule - 26A</t>
+          <t>rule_26a</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9053,7 +9053,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Rule - 26B</t>
+          <t>rule_26b</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9083,7 +9083,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Rule - 26C</t>
+          <t>rule_26c</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Rule - 26D</t>
+          <t>rule_26d</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9143,7 +9143,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Rule - 27</t>
+          <t>rule_27</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9173,7 +9173,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Rule - 28</t>
+          <t>rule_28</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Rule - 28A</t>
+          <t>rule_28a</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9233,7 +9233,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Rule - 28AA</t>
+          <t>rule_28aa</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Rule - 28AB</t>
+          <t>rule_28ab</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9293,7 +9293,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Rule - 29</t>
+          <t>rule_29</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Rule - 29A</t>
+          <t>rule_29a</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9353,7 +9353,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Rule - 29AA</t>
+          <t>rule_29aa</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9383,7 +9383,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Rule - 29B</t>
+          <t>rule_29b</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9413,7 +9413,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Rule - 29BA</t>
+          <t>rule_29ba</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9443,7 +9443,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Rule - 29C</t>
+          <t>rule_29c</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9473,7 +9473,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Rule - 29D</t>
+          <t>rule_29d</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -9503,7 +9503,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Rule - 30</t>
+          <t>rule_30</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Rule - 30A</t>
+          <t>rule_30a</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Rule - 31</t>
+          <t>rule_31</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -9593,7 +9593,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Rule - 31A</t>
+          <t>rule_31a</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -9623,7 +9623,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Rule - 31AA</t>
+          <t>rule_31aa</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -9653,7 +9653,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Rule - 31AB</t>
+          <t>rule_31ab</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -9683,7 +9683,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Rule - 31AC</t>
+          <t>rule_31ac</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -9713,7 +9713,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Rule - 31ACA</t>
+          <t>rule_31aca</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -9743,7 +9743,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Rule - 31ACB</t>
+          <t>rule_31acb</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Rule - 32</t>
+          <t>rule_32</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -9803,7 +9803,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Rule - 33</t>
+          <t>rule_33</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -9833,7 +9833,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Rule - 34</t>
+          <t>rule_34</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Rule - 35</t>
+          <t>rule_35</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -9893,7 +9893,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Rule - 36</t>
+          <t>rule_36</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -9923,7 +9923,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Rule - 36A</t>
+          <t>rule_36a</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -9953,7 +9953,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Rule - 37</t>
+          <t>rule_37</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -9983,7 +9983,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Rule - 37A</t>
+          <t>rule_37a</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10013,7 +10013,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Rule - 37AA</t>
+          <t>rule_37aa</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10043,7 +10043,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Rule - 37B</t>
+          <t>rule_37b</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10073,7 +10073,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Rule - 37BA</t>
+          <t>rule_37ba</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10103,7 +10103,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Rule - 37BB</t>
+          <t>rule_37bb</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10133,7 +10133,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Rule - 37BC</t>
+          <t>rule_37bc</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Rule - 37C</t>
+          <t>rule_37c</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10193,7 +10193,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Rule - 37CA</t>
+          <t>rule_37ca</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10223,7 +10223,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Rule - 37CB</t>
+          <t>rule_37cb</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10253,7 +10253,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Rule - 37D</t>
+          <t>rule_37d</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10283,7 +10283,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Rule - 37E</t>
+          <t>rule_37e</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10313,7 +10313,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Rule - 37EA</t>
+          <t>rule_37ea</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10343,7 +10343,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Rule - 37F</t>
+          <t>rule_37f</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10373,7 +10373,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Rule - 37G</t>
+          <t>rule_37g</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -10403,7 +10403,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Rule - 37H</t>
+          <t>rule_37h</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -10433,7 +10433,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Rule - 37-I</t>
+          <t>rule_37</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
@@ -10463,7 +10463,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>Rule - 37J</t>
+          <t>rule_37j</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
@@ -10493,7 +10493,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Rule - 38</t>
+          <t>rule_38</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
@@ -10523,7 +10523,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Rule - 38A</t>
+          <t>rule_38a</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
@@ -10553,7 +10553,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Rule - 39</t>
+          <t>rule_39</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Rule - 40</t>
+          <t>rule_40</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
@@ -10613,7 +10613,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Rule - 40A</t>
+          <t>rule_40a</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
@@ -10643,7 +10643,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>Rule - 40B</t>
+          <t>rule_40b</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
@@ -10673,7 +10673,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Rule - 40BA</t>
+          <t>rule_40ba</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
@@ -10703,7 +10703,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Rule - 40BB</t>
+          <t>rule_40bb</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
@@ -10733,7 +10733,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Rule - 40C</t>
+          <t>rule_40c</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
@@ -10763,7 +10763,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Rule - 40D</t>
+          <t>rule_40d</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
@@ -10793,7 +10793,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Rule - 40E</t>
+          <t>rule_40e</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
@@ -10823,7 +10823,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Rule - 40F</t>
+          <t>rule_40f</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
@@ -10853,7 +10853,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Rule - 40G</t>
+          <t>rule_40g</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
@@ -10883,7 +10883,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Rule - 41</t>
+          <t>rule_41</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
@@ -10913,7 +10913,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Rule - 42</t>
+          <t>rule_42</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
@@ -10943,7 +10943,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Rule - 43</t>
+          <t>rule_43</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
@@ -10973,7 +10973,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Rule - 44</t>
+          <t>rule_44</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
@@ -11003,7 +11003,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Rule - 44A</t>
+          <t>rule_44a</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
@@ -11033,7 +11033,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Rule - 44B</t>
+          <t>rule_44b</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
@@ -11063,7 +11063,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Rule - 44C</t>
+          <t>rule_44c</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
@@ -11093,7 +11093,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>Rule - 44CA</t>
+          <t>rule_44ca</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
@@ -11123,7 +11123,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>Rule - 44D</t>
+          <t>rule_44d</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
@@ -11153,7 +11153,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>Rule - 44DA</t>
+          <t>rule_44da</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>Rule - 44DAA</t>
+          <t>rule_44daa</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
@@ -11213,7 +11213,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>Rule - 44DAB</t>
+          <t>rule_44dab</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
@@ -11243,7 +11243,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>Rule - 44DAC</t>
+          <t>rule_44dac</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
@@ -11273,7 +11273,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Rule - 44DAD</t>
+          <t>rule_44dad</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
@@ -11303,7 +11303,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Rule - 44E</t>
+          <t>rule_44e</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
@@ -11333,7 +11333,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Rule - 44F</t>
+          <t>rule_44f</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
@@ -11363,7 +11363,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>Rule - 44FA</t>
+          <t>rule_44fa</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
@@ -11393,7 +11393,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>Rule - 44G</t>
+          <t>rule_44g</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
@@ -11423,7 +11423,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Rule - 44GA</t>
+          <t>rule_44ga</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
@@ -11453,7 +11453,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Rule - 44H</t>
+          <t>rule_44h</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
@@ -11483,7 +11483,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Rule - 45</t>
+          <t>rule_45</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Rule - 46</t>
+          <t>rule_46</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
@@ -11543,7 +11543,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Rule - 46A</t>
+          <t>rule_46a</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
@@ -11573,7 +11573,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>Rule - 47</t>
+          <t>rule_47</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
@@ -11603,7 +11603,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>Rule - 48</t>
+          <t>rule_48</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
@@ -11633,7 +11633,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>Rule - 48A</t>
+          <t>rule_48a</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
@@ -11663,7 +11663,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>Rule - 48B</t>
+          <t>rule_48b</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
@@ -11693,7 +11693,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>Rule - 48C</t>
+          <t>rule_48c</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>Rule - 48D</t>
+          <t>rule_48d</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
@@ -11753,7 +11753,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Rule - 48DD</t>
+          <t>rule_48dd</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
@@ -11783,7 +11783,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Rule - 48E</t>
+          <t>rule_48e</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
@@ -11813,7 +11813,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Rule - 48F</t>
+          <t>rule_48f</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
@@ -11843,7 +11843,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Rule - 48G</t>
+          <t>rule_48g</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
@@ -11873,7 +11873,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>Rule - 48H</t>
+          <t>rule_48h</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
@@ -11903,7 +11903,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>Rule - 48-I</t>
+          <t>rule_48</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
@@ -11933,7 +11933,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>Rule - 48J</t>
+          <t>rule_48j</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
@@ -11963,7 +11963,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Rule - 48K</t>
+          <t>rule_48k</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
@@ -11993,7 +11993,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Rule - 48L</t>
+          <t>rule_48l</t>
         </is>
       </c>
       <c r="C386" t="inlineStr">
@@ -12023,7 +12023,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Rule - 49</t>
+          <t>rule_49</t>
         </is>
       </c>
       <c r="C387" t="inlineStr">
@@ -12053,7 +12053,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Rule - 50</t>
+          <t>rule_50</t>
         </is>
       </c>
       <c r="C388" t="inlineStr">
@@ -12083,7 +12083,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Rule - 51</t>
+          <t>rule_51</t>
         </is>
       </c>
       <c r="C389" t="inlineStr">
@@ -12113,7 +12113,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>Rule - 51A</t>
+          <t>rule_51a</t>
         </is>
       </c>
       <c r="C390" t="inlineStr">
@@ -12143,7 +12143,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>Rule - 51B</t>
+          <t>rule_51b</t>
         </is>
       </c>
       <c r="C391" t="inlineStr">
@@ -12173,7 +12173,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Rule - 52</t>
+          <t>rule_52</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
@@ -12203,7 +12203,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Rule - 53</t>
+          <t>rule_53</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
@@ -12233,7 +12233,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Rule - 54</t>
+          <t>rule_54</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
@@ -12263,7 +12263,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Rule - 55</t>
+          <t>rule_55</t>
         </is>
       </c>
       <c r="C395" t="inlineStr">
@@ -12293,7 +12293,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Rule - 56</t>
+          <t>rule_56</t>
         </is>
       </c>
       <c r="C396" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Rule - 57</t>
+          <t>rule_57</t>
         </is>
       </c>
       <c r="C397" t="inlineStr">
@@ -12353,7 +12353,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Rule - 58</t>
+          <t>rule_58</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -12383,7 +12383,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Rule - 59</t>
+          <t>rule_59</t>
         </is>
       </c>
       <c r="C399" t="inlineStr">
@@ -12413,7 +12413,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Rule - 60</t>
+          <t>rule_60</t>
         </is>
       </c>
       <c r="C400" t="inlineStr">
@@ -12443,7 +12443,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Rule - 61</t>
+          <t>rule_61</t>
         </is>
       </c>
       <c r="C401" t="inlineStr">
@@ -12473,7 +12473,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Rule - 62</t>
+          <t>rule_62</t>
         </is>
       </c>
       <c r="C402" t="inlineStr">
@@ -12503,7 +12503,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Rule - 63</t>
+          <t>rule_63</t>
         </is>
       </c>
       <c r="C403" t="inlineStr">
@@ -12533,7 +12533,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Rule - 64</t>
+          <t>rule_64</t>
         </is>
       </c>
       <c r="C404" t="inlineStr">
@@ -12563,7 +12563,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Rule - 65</t>
+          <t>rule_65</t>
         </is>
       </c>
       <c r="C405" t="inlineStr">
@@ -12593,7 +12593,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Rule - 66</t>
+          <t>rule_66</t>
         </is>
       </c>
       <c r="C406" t="inlineStr">
@@ -12623,7 +12623,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Rule - 67</t>
+          <t>rule_67</t>
         </is>
       </c>
       <c r="C407" t="inlineStr">
@@ -12653,7 +12653,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Rule - 67A</t>
+          <t>rule_67a</t>
         </is>
       </c>
       <c r="C408" t="inlineStr">
@@ -12683,7 +12683,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Rule - 68</t>
+          <t>rule_68</t>
         </is>
       </c>
       <c r="C409" t="inlineStr">
@@ -12713,7 +12713,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Rule - 69</t>
+          <t>rule_69</t>
         </is>
       </c>
       <c r="C410" t="inlineStr">
@@ -12743,7 +12743,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Rule - 70</t>
+          <t>rule_70</t>
         </is>
       </c>
       <c r="C411" t="inlineStr">
@@ -12773,7 +12773,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Rule - 71</t>
+          <t>rule_71</t>
         </is>
       </c>
       <c r="C412" t="inlineStr">
@@ -12803,7 +12803,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Rule - 71A</t>
+          <t>rule_71a</t>
         </is>
       </c>
       <c r="C413" t="inlineStr">
@@ -12833,7 +12833,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Rule - 72</t>
+          <t>rule_72</t>
         </is>
       </c>
       <c r="C414" t="inlineStr">
@@ -12863,7 +12863,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>Rule - 73</t>
+          <t>rule_73</t>
         </is>
       </c>
       <c r="C415" t="inlineStr">
@@ -12893,7 +12893,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Rule - 74</t>
+          <t>rule_74</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
@@ -12923,7 +12923,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>Rule - 75</t>
+          <t>rule_75</t>
         </is>
       </c>
       <c r="C417" t="inlineStr">
@@ -12953,7 +12953,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>Rule - 76</t>
+          <t>rule_76</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
@@ -12983,7 +12983,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>Rule - 77</t>
+          <t>rule_77</t>
         </is>
       </c>
       <c r="C419" t="inlineStr">
@@ -13013,7 +13013,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>Rule - 78</t>
+          <t>rule_78</t>
         </is>
       </c>
       <c r="C420" t="inlineStr">
@@ -13043,7 +13043,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Rule - 79</t>
+          <t>rule_79</t>
         </is>
       </c>
       <c r="C421" t="inlineStr">
@@ -13073,7 +13073,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>Rule - 80</t>
+          <t>rule_80</t>
         </is>
       </c>
       <c r="C422" t="inlineStr">
@@ -13103,7 +13103,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>Rule - 81</t>
+          <t>rule_81</t>
         </is>
       </c>
       <c r="C423" t="inlineStr">
@@ -13133,7 +13133,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>Rule - 82</t>
+          <t>rule_82</t>
         </is>
       </c>
       <c r="C424" t="inlineStr">
@@ -13163,7 +13163,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>Rule - 83</t>
+          <t>rule_83</t>
         </is>
       </c>
       <c r="C425" t="inlineStr">
@@ -13193,7 +13193,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>Rule - 84</t>
+          <t>rule_84</t>
         </is>
       </c>
       <c r="C426" t="inlineStr">
@@ -13223,7 +13223,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>Rule - 85</t>
+          <t>rule_85</t>
         </is>
       </c>
       <c r="C427" t="inlineStr">
@@ -13253,7 +13253,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>Rule - 86</t>
+          <t>rule_86</t>
         </is>
       </c>
       <c r="C428" t="inlineStr">
@@ -13283,7 +13283,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Rule - 87</t>
+          <t>rule_87</t>
         </is>
       </c>
       <c r="C429" t="inlineStr">
@@ -13313,7 +13313,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>Rule - 88</t>
+          <t>rule_88</t>
         </is>
       </c>
       <c r="C430" t="inlineStr">
@@ -13343,7 +13343,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>Rule - 89</t>
+          <t>rule_89</t>
         </is>
       </c>
       <c r="C431" t="inlineStr">
@@ -13373,7 +13373,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>Rule - 90</t>
+          <t>rule_90</t>
         </is>
       </c>
       <c r="C432" t="inlineStr">
@@ -13403,7 +13403,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>Rule - 91</t>
+          <t>rule_91</t>
         </is>
       </c>
       <c r="C433" t="inlineStr">
@@ -13433,7 +13433,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>Rule - 92</t>
+          <t>rule_92</t>
         </is>
       </c>
       <c r="C434" t="inlineStr">
@@ -13463,7 +13463,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>Rule - 93</t>
+          <t>rule_93</t>
         </is>
       </c>
       <c r="C435" t="inlineStr">
@@ -13493,7 +13493,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>Rule - 94</t>
+          <t>rule_94</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
@@ -13523,7 +13523,7 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>Rule - 95</t>
+          <t>rule_95</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
@@ -13553,7 +13553,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>Rule - 96</t>
+          <t>rule_96</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
@@ -13583,7 +13583,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>Rule - 97</t>
+          <t>rule_97</t>
         </is>
       </c>
       <c r="C439" t="inlineStr">
@@ -13613,7 +13613,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>Rule - 98</t>
+          <t>rule_98</t>
         </is>
       </c>
       <c r="C440" t="inlineStr">
@@ -13643,7 +13643,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>Rule - 99</t>
+          <t>rule_99</t>
         </is>
       </c>
       <c r="C441" t="inlineStr">
@@ -13673,7 +13673,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>Rule - 100</t>
+          <t>rule_100</t>
         </is>
       </c>
       <c r="C442" t="inlineStr">
@@ -13703,7 +13703,7 @@
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>Rule - 101</t>
+          <t>rule_101</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
@@ -13733,7 +13733,7 @@
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>Rule - 101A</t>
+          <t>rule_101a</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
@@ -13763,7 +13763,7 @@
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>Rule - 102</t>
+          <t>rule_102</t>
         </is>
       </c>
       <c r="C445" t="inlineStr">
@@ -13793,7 +13793,7 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>Rule - 103</t>
+          <t>rule_103</t>
         </is>
       </c>
       <c r="C446" t="inlineStr">
@@ -13823,7 +13823,7 @@
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>Rule - 104</t>
+          <t>rule_104</t>
         </is>
       </c>
       <c r="C447" t="inlineStr">
@@ -13853,7 +13853,7 @@
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>Rule - 105</t>
+          <t>rule_105</t>
         </is>
       </c>
       <c r="C448" t="inlineStr">
@@ -13883,7 +13883,7 @@
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>Rule - 106</t>
+          <t>rule_106</t>
         </is>
       </c>
       <c r="C449" t="inlineStr">
@@ -13913,7 +13913,7 @@
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>Rule - 107</t>
+          <t>rule_107</t>
         </is>
       </c>
       <c r="C450" t="inlineStr">
@@ -13943,7 +13943,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>Rule - 108</t>
+          <t>rule_108</t>
         </is>
       </c>
       <c r="C451" t="inlineStr">
@@ -13973,7 +13973,7 @@
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>Rule - 109</t>
+          <t>rule_109</t>
         </is>
       </c>
       <c r="C452" t="inlineStr">
@@ -14003,7 +14003,7 @@
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>Rule - 110</t>
+          <t>rule_110</t>
         </is>
       </c>
       <c r="C453" t="inlineStr">
@@ -14033,7 +14033,7 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>Rule - 111</t>
+          <t>rule_111</t>
         </is>
       </c>
       <c r="C454" t="inlineStr">
@@ -14063,7 +14063,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>Rule - 111A</t>
+          <t>rule_111a</t>
         </is>
       </c>
       <c r="C455" t="inlineStr">
@@ -14093,7 +14093,7 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>Rule - 111AA</t>
+          <t>rule_111aa</t>
         </is>
       </c>
       <c r="C456" t="inlineStr">
@@ -14123,7 +14123,7 @@
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>Rule - 111AB</t>
+          <t>rule_111ab</t>
         </is>
       </c>
       <c r="C457" t="inlineStr">
@@ -14153,7 +14153,7 @@
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>Rule - 111B</t>
+          <t>rule_111b</t>
         </is>
       </c>
       <c r="C458" t="inlineStr">
@@ -14183,7 +14183,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>Rule - 112</t>
+          <t>rule_112</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
@@ -14213,7 +14213,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>Rule - 112A</t>
+          <t>rule_112a</t>
         </is>
       </c>
       <c r="C460" t="inlineStr">
@@ -14243,7 +14243,7 @@
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>Rule - 112B</t>
+          <t>rule_112b</t>
         </is>
       </c>
       <c r="C461" t="inlineStr">
@@ -14273,7 +14273,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>Rule - 112C</t>
+          <t>rule_112c</t>
         </is>
       </c>
       <c r="C462" t="inlineStr">
@@ -14303,7 +14303,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>Rule - 112D</t>
+          <t>rule_112d</t>
         </is>
       </c>
       <c r="C463" t="inlineStr">
@@ -14333,7 +14333,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>Rule - 112E</t>
+          <t>rule_112e</t>
         </is>
       </c>
       <c r="C464" t="inlineStr">
@@ -14363,7 +14363,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>Rule - 112F</t>
+          <t>rule_112f</t>
         </is>
       </c>
       <c r="C465" t="inlineStr">
@@ -14393,7 +14393,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>Rule - 113</t>
+          <t>rule_113</t>
         </is>
       </c>
       <c r="C466" t="inlineStr">
@@ -14423,7 +14423,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>Rule - 114</t>
+          <t>rule_114</t>
         </is>
       </c>
       <c r="C467" t="inlineStr">
@@ -14453,7 +14453,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>Rule - 114A</t>
+          <t>rule_114a</t>
         </is>
       </c>
       <c r="C468" t="inlineStr">
@@ -14483,7 +14483,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>Rule - 114AA</t>
+          <t>rule_114aa</t>
         </is>
       </c>
       <c r="C469" t="inlineStr">
@@ -14513,7 +14513,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>Rule - 114AAA</t>
+          <t>rule_114aaa</t>
         </is>
       </c>
       <c r="C470" t="inlineStr">
@@ -14543,7 +14543,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Rule - 114AAB</t>
+          <t>rule_114aab</t>
         </is>
       </c>
       <c r="C471" t="inlineStr">
@@ -14573,7 +14573,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>Rule - 114B</t>
+          <t>rule_114b</t>
         </is>
       </c>
       <c r="C472" t="inlineStr">
@@ -14603,7 +14603,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>Rule - 114BA</t>
+          <t>rule_114ba</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -14633,7 +14633,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>Rule - 114BB</t>
+          <t>rule_114bb</t>
         </is>
       </c>
       <c r="C474" t="inlineStr">
@@ -14663,7 +14663,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>Rule - 114C</t>
+          <t>rule_114c</t>
         </is>
       </c>
       <c r="C475" t="inlineStr">
@@ -14693,7 +14693,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>Rule - 114D</t>
+          <t>rule_114d</t>
         </is>
       </c>
       <c r="C476" t="inlineStr">
@@ -14723,7 +14723,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>Rule - 114DA</t>
+          <t>rule_114da</t>
         </is>
       </c>
       <c r="C477" t="inlineStr">
@@ -14753,7 +14753,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>Rule - 114DB</t>
+          <t>rule_114db</t>
         </is>
       </c>
       <c r="C478" t="inlineStr">
@@ -14783,7 +14783,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>Rule - 114E</t>
+          <t>rule_114e</t>
         </is>
       </c>
       <c r="C479" t="inlineStr">
@@ -14813,7 +14813,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>Rule - 114F</t>
+          <t>rule_114f</t>
         </is>
       </c>
       <c r="C480" t="inlineStr">
@@ -14843,7 +14843,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>Rule - 114G</t>
+          <t>rule_114g</t>
         </is>
       </c>
       <c r="C481" t="inlineStr">
@@ -14873,7 +14873,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>Rule - 114H</t>
+          <t>rule_114h</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
@@ -14903,7 +14903,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>Rule - 114-I</t>
+          <t>rule_114</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
@@ -14933,7 +14933,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>Rule - 115</t>
+          <t>rule_115</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>Rule - 115A</t>
+          <t>rule_115a</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
@@ -14993,7 +14993,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Rule - 116</t>
+          <t>rule_116</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
@@ -15023,7 +15023,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Rule - 117</t>
+          <t>rule_117</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
@@ -15053,7 +15053,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Rule - 117A</t>
+          <t>rule_117a</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
@@ -15083,7 +15083,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Rule - 117B</t>
+          <t>rule_117b</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
@@ -15113,7 +15113,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>Rule - 117C</t>
+          <t>rule_117c</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
@@ -15143,7 +15143,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>Rule - 118</t>
+          <t>rule_118</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
@@ -15173,7 +15173,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Rule - 119</t>
+          <t>rule_119</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
@@ -15203,7 +15203,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>Rule - 119A</t>
+          <t>rule_119a</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -15233,7 +15233,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>Rule - 119AA</t>
+          <t>rule_119aa</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
@@ -15263,7 +15263,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>Rule - 120</t>
+          <t>rule_120</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
@@ -15293,7 +15293,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>Rule - 121</t>
+          <t>rule_121</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
@@ -15323,7 +15323,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>Rule - 121A</t>
+          <t>rule_121a</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
@@ -15353,7 +15353,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Rule - 122</t>
+          <t>rule_122</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
@@ -15383,7 +15383,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>Rule - 123</t>
+          <t>rule_123</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
@@ -15413,7 +15413,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Rule - 124</t>
+          <t>rule_124</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
@@ -15443,7 +15443,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>Rule - 125</t>
+          <t>rule_125</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
@@ -15473,7 +15473,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Rule - 126</t>
+          <t>rule_126</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
@@ -15503,7 +15503,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Rule - 127</t>
+          <t>rule_127</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
@@ -15533,7 +15533,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>Rule - 127A</t>
+          <t>rule_127a</t>
         </is>
       </c>
       <c r="C504" t="inlineStr">
@@ -15563,7 +15563,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Rule - 128</t>
+          <t>rule_128</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
@@ -15593,7 +15593,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Rule - 129</t>
+          <t>rule_129</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
@@ -15623,7 +15623,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>Rule - 130</t>
+          <t>rule_130</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
@@ -15653,7 +15653,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Rule - 131</t>
+          <t>rule_131</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>Rule - 132</t>
+          <t>rule_132</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -15713,7 +15713,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Rule - 133</t>
+          <t>rule_133</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -15743,7 +15743,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Rule - 134</t>
+          <t>rule_134</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
@@ -15773,7 +15773,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Rule - NEW APPENDIX I</t>
+          <t>rule_new</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
@@ -15803,7 +15803,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Rule - OLD APPENDIX I</t>
+          <t>rule_old</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
@@ -15833,7 +15833,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>Rule - OLD APPENDIX I</t>
+          <t>rule_old</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
@@ -15863,7 +15863,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>Rule - OLD APPENDIX I</t>
+          <t>rule_old</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
@@ -15893,7 +15893,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Rule - APPENDIX IA</t>
+          <t>rule_appendix</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
@@ -15923,7 +15923,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>Rule - APPENDIX II</t>
+          <t>rule_appendix</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
@@ -15953,7 +15953,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>Rule - APPENDIX III</t>
+          <t>rule_appendix</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
@@ -15983,7 +15983,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>Rule - APPENDIX IV</t>
+          <t>rule_appendix</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">

</xml_diff>